<commit_message>
I added my homework
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Book1.xlsx
+++ b/src/test/resources/testdata/Book1.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335"/>
+    <workbookView windowWidth="14975" windowHeight="7055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddReport" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:E3"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>FirstName</t>
   </si>
@@ -44,7 +45,7 @@
     <t>Barindik</t>
   </si>
   <si>
-    <t>reyhane@gamil.com</t>
+    <t>reyhanee@gamil.com</t>
   </si>
   <si>
     <t>njfjffbf@</t>
@@ -59,7 +60,7 @@
     <t>Yakut</t>
   </si>
   <si>
-    <t>yunusss@gmail.com</t>
+    <t>yunusssu@gmail.com</t>
   </si>
   <si>
     <t>jhskjfhjk@</t>
@@ -74,7 +75,7 @@
     <t>Inci</t>
   </si>
   <si>
-    <t>gulsuminic@gamil.com</t>
+    <t>gulsuminiic@gamil.com</t>
   </si>
   <si>
     <t>jhffgfhg#@</t>
@@ -89,7 +90,7 @@
     <t>Duman</t>
   </si>
   <si>
-    <t>senelDuman@gmail.com</t>
+    <t>senelDumann@gmail.com</t>
   </si>
   <si>
     <t>hfsjkhfh$#</t>
@@ -101,10 +102,64 @@
     <t>Dogruer</t>
   </si>
   <si>
-    <t>turkerdogruer@gmail.com</t>
+    <t>turkerdogrueeer@gmail.com</t>
   </si>
   <si>
     <t>jbkjvjbjvkjj@</t>
+  </si>
+  <si>
+    <t>ReportName</t>
+  </si>
+  <si>
+    <t>Selection Critaria</t>
+  </si>
+  <si>
+    <t>Selected Critaria Include</t>
+  </si>
+  <si>
+    <t>Display Field Groups</t>
+  </si>
+  <si>
+    <t>Display Fields</t>
+  </si>
+  <si>
+    <t>Canvas Group</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>CurrentEmployeesOnly</t>
+  </si>
+  <si>
+    <t>Languages</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>My Project</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>Employee Id</t>
+  </si>
+  <si>
+    <t>Our Team Project</t>
+  </si>
+  <si>
+    <t>Skill</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Pay Grade</t>
   </si>
 </sst>
 </file>
@@ -114,8 +169,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -128,6 +183,14 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -135,6 +198,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -142,14 +212,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -157,7 +220,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -172,52 +235,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,42 +279,49 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -279,187 +334,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -470,30 +525,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -514,10 +545,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -547,11 +576,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -570,12 +616,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -593,138 +648,141 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1049,12 +1107,12 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="5"/>
   <cols>
-    <col min="4" max="4" width="13.2222222222222" customWidth="1"/>
+    <col min="4" max="4" width="25.4444444444444" customWidth="1"/>
     <col min="5" max="5" width="13.5555555555556" customWidth="1"/>
     <col min="6" max="6" width="11.3333333333333" customWidth="1"/>
   </cols>
@@ -1109,7 +1167,7 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E3" t="s">
@@ -1129,7 +1187,7 @@
       <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E4" t="s">
@@ -1169,7 +1227,7 @@
       <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E6" t="s">
@@ -1181,13 +1239,106 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="reyhane@gamil.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="yunusss@gmail.com"/>
-    <hyperlink ref="D4" r:id="rId3" display="gulsuminic@gamil.com"/>
-    <hyperlink ref="D5" r:id="rId4" display="senelDuman@gmail.com"/>
-    <hyperlink ref="D6" r:id="rId5" display="turkerdogruer@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="reyhanee@gamil.com" tooltip="mailto:reyhanee@gamil.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="yunusssu@gmail.com" tooltip="mailto:yunusssu@gmail.com"/>
+    <hyperlink ref="D4" r:id="rId3" display="gulsuminiic@gamil.com" tooltip="mailto:gulsuminiic@gamil.com"/>
+    <hyperlink ref="D5" r:id="rId4" display="senelDumann@gmail.com" tooltip="mailto:senelDumann@gmail.com"/>
+    <hyperlink ref="D6" r:id="rId5" display="turkerdogrueeer@gmail.com" tooltip="mailto:turkerdogrueeer@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="14.8888888888889" customWidth="1"/>
+    <col min="2" max="2" width="15.5555555555556" customWidth="1"/>
+    <col min="3" max="3" width="21.5555555555556" customWidth="1"/>
+    <col min="4" max="4" width="17.8888888888889" customWidth="1"/>
+    <col min="5" max="5" width="13.4444444444444" customWidth="1"/>
+    <col min="6" max="6" width="14.5555555555556" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>